<commit_message>
Removed b2b question per BL-197
Removed b2b question and updated VIDs covered by automation, per BL-197
</commit_message>
<xml_diff>
--- a/TestCaseData/TestCaseData_businessloan.xlsx
+++ b/TestCaseData/TestCaseData_businessloan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="109">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -270,9 +270,6 @@
     <t>b2_04_PersonalCrossSell</t>
   </si>
   <si>
-    <t>0-0-0-0-1-0-0</t>
-  </si>
-  <si>
     <t>LendingTree Testing Partnership</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>Prod_bl_01</t>
   </si>
   <si>
-    <t>0-0-5-0-0-1-1-0-0</t>
-  </si>
-  <si>
     <t>bl_04_PersonalCrossSell</t>
   </si>
   <si>
@@ -340,6 +334,18 @@
   </si>
   <si>
     <t>1111</t>
+  </si>
+  <si>
+    <t>0-0-0-0-1-2-0</t>
+  </si>
+  <si>
+    <t>0-0-0-0-0-2-0</t>
+  </si>
+  <si>
+    <t>0-0-5-0-0-1-2-0-0</t>
+  </si>
+  <si>
+    <t>0-0-5-0-0-0-2-0-0</t>
   </si>
 </sst>
 </file>
@@ -684,9 +690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -818,11 +822,14 @@
       <c r="D2" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>54</v>
@@ -892,11 +899,14 @@
       <c r="D3" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="F3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>55</v>
@@ -966,11 +976,14 @@
       <c r="D4" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E4" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>56</v>
@@ -1015,13 +1028,13 @@
         <v>21</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>38</v>
@@ -1041,13 +1054,13 @@
         <v>52</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>40</v>
@@ -1071,13 +1084,13 @@
         <v>19</v>
       </c>
       <c r="O5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="R5" s="1" t="s">
         <v>72</v>
@@ -1117,11 +1130,14 @@
       <c r="D6" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>40</v>
@@ -1191,11 +1207,14 @@
       <c r="D7" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="E7" t="s">
+        <v>106</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>40</v>
@@ -1254,7 +1273,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>45</v>
@@ -1263,19 +1282,22 @@
         <v>43</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>61</v>
@@ -1328,7 +1350,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>45</v>
@@ -1337,16 +1359,19 @@
         <v>43</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>46</v>
@@ -1402,7 +1427,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>45</v>
@@ -1411,19 +1436,22 @@
         <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>107</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>60</v>
@@ -1462,13 +1490,13 @@
         <v>21</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>38</v>
@@ -1476,7 +1504,7 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>45</v>
@@ -1485,19 +1513,19 @@
         <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>46</v>
@@ -1518,13 +1546,13 @@
         <v>19</v>
       </c>
       <c r="O11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="R11" s="1" t="s">
         <v>72</v>
@@ -1553,25 +1581,28 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E12" t="s">
+        <v>108</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>46</v>
@@ -1627,25 +1658,28 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
+      </c>
+      <c r="E13" t="s">
+        <v>108</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>46</v>

</xml_diff>